<commit_message>
fix bug template import
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_stock/static/src/xlsx/template_update_nhap_kho.xlsx
+++ b/addons/custom/forlife_stock/static/src/xlsx/template_update_nhap_kho.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Project\m_onnet_odoo_mfl2201er\addons\custom\forlife_stock\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B28193-CAA1-4510-8E86-8708109C0F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFD711D-B7B9-4FCD-9D62-382C44A7889A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F89CA616-5065-4975-8C45-011712555742}"/>
   </bookViews>
@@ -27,15 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
-    <t>Mã phiếu</t>
-  </si>
-  <si>
-    <t>Hoạt động không có trong gói hàng / Sản phẩm</t>
-  </si>
-  <si>
-    <t>Ngày hoàn thành</t>
-  </si>
-  <si>
     <t>1521_NPL</t>
   </si>
   <si>
@@ -45,17 +36,91 @@
     <t>1077/IN/00170</t>
   </si>
   <si>
-    <t>Hoạt động không có trong gói hàng / STT dòng</t>
-  </si>
-  <si>
-    <t>Hoạt động không có trong gói hàng / Số lượng mua hoàn thành</t>
+    <r>
+      <t xml:space="preserve">Ngày hoàn thành </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã phiếu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hoạt động không có trong gói hàng / STT dòng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hoạt động không có trong gói hàng / Sản phẩm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hoạt động không có trong gói hàng / Số lượng mua hoàn thành</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (*)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +133,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -117,15 +198,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,32 +525,32 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.21875" customWidth="1"/>
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -477,13 +559,13 @@
         <v>45265</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>88</v>
@@ -494,13 +576,13 @@
         <v>45265</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>11</v>

</xml_diff>